<commit_message>
test case sign in documented
</commit_message>
<xml_diff>
--- a/com.apartments/src/test/resources/test_data.xlsx
+++ b/com.apartments/src/test/resources/test_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A9E0EE-B5F6-4DEB-B310-AB32ACBBCBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6884A5AF-59BA-4324-8229-AEC99B82C8D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>Email</t>
   </si>
@@ -57,6 +57,18 @@
   </si>
   <si>
     <t>AydenLiam1213</t>
+  </si>
+  <si>
+    <t>abctestemail4!!!!@gmail.com</t>
+  </si>
+  <si>
+    <t>abctestemail1$@gmail.com</t>
+  </si>
+  <si>
+    <t>abctestemail3$@gmail.com</t>
+  </si>
+  <si>
+    <t>james.corley@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -494,7 +506,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -521,49 +533,48 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="QqwertyQ@123!" xr:uid="{429AEC22-2A7D-41D1-BEEC-366D56F58E46}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{E1D422F6-BB11-4669-98CC-C9FE14F78322}"/>
-    <hyperlink ref="A6" r:id="rId3" xr:uid="{7153B564-111F-433C-83F0-D036529A0348}"/>
-    <hyperlink ref="A2:A5" r:id="rId4" display="abctestemail237!!@gmail.com" xr:uid="{0FFD8762-3E94-40D5-A492-71CC8771AF28}"/>
-    <hyperlink ref="A2" r:id="rId5" xr:uid="{04803DC0-ED29-4AB8-A6E0-D889F7E5DD99}"/>
-    <hyperlink ref="A3" r:id="rId6" xr:uid="{DDD1A662-298D-4DFD-AB8B-D5FBF8AFCADB}"/>
-    <hyperlink ref="A4" r:id="rId7" xr:uid="{16B6CB8B-815F-4F1E-A5E8-70C68FEF68F2}"/>
-    <hyperlink ref="A5" r:id="rId8" xr:uid="{CFD60770-CC08-4A55-B6DA-05857299C7F6}"/>
+    <hyperlink ref="A6" r:id="rId2" xr:uid="{7153B564-111F-433C-83F0-D036529A0348}"/>
+    <hyperlink ref="A2:A5" r:id="rId3" display="abctestemail237!!@gmail.com" xr:uid="{0FFD8762-3E94-40D5-A492-71CC8771AF28}"/>
+    <hyperlink ref="A2" r:id="rId4" xr:uid="{04803DC0-ED29-4AB8-A6E0-D889F7E5DD99}"/>
+    <hyperlink ref="A3" r:id="rId5" xr:uid="{DDD1A662-298D-4DFD-AB8B-D5FBF8AFCADB}"/>
+    <hyperlink ref="A4" r:id="rId6" xr:uid="{16B6CB8B-815F-4F1E-A5E8-70C68FEF68F2}"/>
+    <hyperlink ref="A5" r:id="rId7" xr:uid="{CFD60770-CC08-4A55-B6DA-05857299C7F6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
test account settings completed
</commit_message>
<xml_diff>
--- a/com.apartments/src/test/resources/test_data.xlsx
+++ b/com.apartments/src/test/resources/test_data.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE96212-A525-4330-ADC8-347D48BA43C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AABC7A-1BBF-48FD-ABCD-02D2F1F30965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3216" yWindow="7728" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3324" yWindow="3504" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="signin" sheetId="2" r:id="rId1"/>
     <sheet name="doSignIn" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="doSaveUpdates" sheetId="5" r:id="rId3"/>
     <sheet name="doSearch" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>Email</t>
   </si>
@@ -81,6 +81,33 @@
   </si>
   <si>
     <t>19104 PA,Philadelphia</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>streetAddress</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>125 Main st</t>
+  </si>
+  <si>
+    <t>123 Main st</t>
+  </si>
+  <si>
+    <t>124 Main st</t>
+  </si>
+  <si>
+    <t>Philadelphia</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Pitsburgh</t>
   </si>
 </sst>
 </file>
@@ -437,7 +464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -503,11 +530,11 @@
     <hyperlink ref="B4" r:id="rId4" xr:uid="{A2D57DA5-F57B-4EC0-9B60-86091CC06684}"/>
     <hyperlink ref="B5" r:id="rId5" xr:uid="{092947D6-816E-4A87-86C1-6444F869D5E6}"/>
     <hyperlink ref="B6" r:id="rId6" xr:uid="{334C9F71-A274-4C0A-B827-F4D506A14ABF}"/>
-    <hyperlink ref="A2:A5" r:id="rId7" display="abctestemail237!!@gmail.com" xr:uid="{76FE5A68-8A16-4235-8B37-785AB4804E90}"/>
-    <hyperlink ref="A2" r:id="rId8" xr:uid="{BF33BD21-C36E-4BF5-8837-82B17F81FB17}"/>
-    <hyperlink ref="A3" r:id="rId9" xr:uid="{5DCB839A-62CC-4149-89BF-11A0CBAC0BC0}"/>
-    <hyperlink ref="A4" r:id="rId10" xr:uid="{6DC029EA-4096-45AF-9C95-C50D66D2F7A8}"/>
-    <hyperlink ref="A5" r:id="rId11" xr:uid="{8ED416A2-7413-4071-B44D-BE3896560478}"/>
+    <hyperlink ref="A3" r:id="rId7" xr:uid="{5DCB839A-62CC-4149-89BF-11A0CBAC0BC0}"/>
+    <hyperlink ref="A4" r:id="rId8" xr:uid="{6DC029EA-4096-45AF-9C95-C50D66D2F7A8}"/>
+    <hyperlink ref="A5" r:id="rId9" xr:uid="{8ED416A2-7413-4071-B44D-BE3896560478}"/>
+    <hyperlink ref="A2" r:id="rId10" xr:uid="{BF33BD21-C36E-4BF5-8837-82B17F81FB17}"/>
+    <hyperlink ref="A2:A5" r:id="rId11" display="abctestemail237!!@gmail.com" xr:uid="{76FE5A68-8A16-4235-8B37-785AB4804E90}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -517,7 +544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -594,12 +621,63 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C159359-5032-458D-AEEB-0A56F13FFA5A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2679875852</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2678526547</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2674718956</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>